<commit_message>
Creación de archivo de pruebas con selenium IDE
</commit_message>
<xml_diff>
--- a/#1_SAUCEDEMO/suit_de_pruebas.xlsx
+++ b/#1_SAUCEDEMO/suit_de_pruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Desktop\QA_1_SAUCEDEMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Desktop\qa-practice\#1_SAUCEDEMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D769C450-AAC4-4EB9-936D-AE381E185B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61709B13-D15E-4AE2-A99F-8FD6D95FD99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{AFCFE919-6E85-4DC5-AA7B-67DF6236A715}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{AFCFE919-6E85-4DC5-AA7B-67DF6236A715}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="3" r:id="rId1"/>
@@ -2342,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C466D41-D5C6-4D27-967C-822F08B8CB78}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2382,7 +2382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -2481,8 +2481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B6585B-6B35-44C0-849D-CC5D2662B9BF}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>